<commit_message>
Chỉnh sửa giao diện CRUD giảng viên
</commit_message>
<xml_diff>
--- a/public/file/import-lecturer.xlsx
+++ b/public/file/import-lecturer.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Họ và tên</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Chức vị</t>
   </si>
   <si>
-    <t>HTTT</t>
-  </si>
-  <si>
     <t>TestImport1</t>
   </si>
   <si>
@@ -71,27 +68,56 @@
     <t>testimport4@gmail.com</t>
   </si>
   <si>
-    <t>CNTT</t>
-  </si>
-  <si>
     <t>Thạc sĩ</t>
   </si>
   <si>
     <t>Tiến sĩ</t>
   </si>
   <si>
-    <t>KTPM</t>
-  </si>
-  <si>
     <t>Trưởng khoa</t>
+  </si>
+  <si>
+    <t>Số điện thoại</t>
+  </si>
+  <si>
+    <t>0969615123</t>
+  </si>
+  <si>
+    <t>0969615456</t>
+  </si>
+  <si>
+    <t>0969615789</t>
+  </si>
+  <si>
+    <t>0969615246</t>
+  </si>
+  <si>
+    <t>Hệ thống thông tin</t>
+  </si>
+  <si>
+    <t>Kỹ thuật phần mềm</t>
+  </si>
+  <si>
+    <t>Công nghệ thông tin</t>
+  </si>
+  <si>
+    <t>Trí tuệ nhân tạo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -126,11 +152,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -412,102 +440,124 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
     </row>
   </sheetData>
@@ -519,5 +569,6 @@
     <hyperlink ref="B5" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sửa import sinh viên, giảng viên
</commit_message>
<xml_diff>
--- a/public/file/import-lecturer.xlsx
+++ b/public/file/import-lecturer.xlsx
@@ -44,30 +44,6 @@
     <t>Chức vị</t>
   </si>
   <si>
-    <t>TestImport1</t>
-  </si>
-  <si>
-    <t>TestImport2</t>
-  </si>
-  <si>
-    <t>TestImport3</t>
-  </si>
-  <si>
-    <t>TestImport4</t>
-  </si>
-  <si>
-    <t>testimport1@gmail.com</t>
-  </si>
-  <si>
-    <t>testimport2@gmail.com</t>
-  </si>
-  <si>
-    <t>testimport3@gmail.com</t>
-  </si>
-  <si>
-    <t>testimport4@gmail.com</t>
-  </si>
-  <si>
     <t>Thạc sĩ</t>
   </si>
   <si>
@@ -104,42 +80,6 @@
     <t>Trí tuệ nhân tạo</t>
   </si>
   <si>
-    <t>TestImport5</t>
-  </si>
-  <si>
-    <t>TestImport6</t>
-  </si>
-  <si>
-    <t>TestImport7</t>
-  </si>
-  <si>
-    <t>TestImport8</t>
-  </si>
-  <si>
-    <t>TestImport9</t>
-  </si>
-  <si>
-    <t>TestImport10</t>
-  </si>
-  <si>
-    <t>testimport5@gmail.com</t>
-  </si>
-  <si>
-    <t>testimport7@gmail.com</t>
-  </si>
-  <si>
-    <t>testimport8@gmail.com</t>
-  </si>
-  <si>
-    <t>testimport9@gmail.com</t>
-  </si>
-  <si>
-    <t>testimport10@gmail.com</t>
-  </si>
-  <si>
-    <t>testimport6@gmail.com</t>
-  </si>
-  <si>
     <t>0969615247</t>
   </si>
   <si>
@@ -156,6 +96,66 @@
   </si>
   <si>
     <t>0969615252</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn A</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn B</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn C</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn D</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn E</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị G</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị H</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị I</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị J</t>
+  </si>
+  <si>
+    <t>Nguyễn Thị K</t>
+  </si>
+  <si>
+    <t>gv1@tlu.edu.vn</t>
+  </si>
+  <si>
+    <t>gv2@tlu.edu.vn</t>
+  </si>
+  <si>
+    <t>gv3@tlu.edu.vn</t>
+  </si>
+  <si>
+    <t>gv4@tlu.edu.vn</t>
+  </si>
+  <si>
+    <t>gv5@tlu.edu.vn</t>
+  </si>
+  <si>
+    <t>gv6@tlu.edu.vn</t>
+  </si>
+  <si>
+    <t>gv7@tlu.edu.vn</t>
+  </si>
+  <si>
+    <t>gv8@tlu.edu.vn</t>
+  </si>
+  <si>
+    <t>gv9@tlu.edu.vn</t>
+  </si>
+  <si>
+    <t>gv10@tlu.edu.vn</t>
   </si>
 </sst>
 </file>
@@ -498,12 +498,12 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
@@ -520,7 +520,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -537,211 +537,208 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B5:B9" r:id="rId4" display="testimport3@gmail.com"/>
-    <hyperlink ref="B4" r:id="rId5"/>
-    <hyperlink ref="B7:B11" r:id="rId6" display="testimport3@gmail.com"/>
-    <hyperlink ref="B6" r:id="rId7"/>
-    <hyperlink ref="B7" r:id="rId8"/>
-    <hyperlink ref="B8" r:id="rId9"/>
-    <hyperlink ref="B9" r:id="rId10"/>
-    <hyperlink ref="B10" r:id="rId11"/>
-    <hyperlink ref="B11" r:id="rId12"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B5" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B7" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId7"/>
+    <hyperlink ref="B9" r:id="rId8"/>
+    <hyperlink ref="B10" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>